<commit_message>
Updated requirements to cover behavior for duplicates
</commit_message>
<xml_diff>
--- a/doc/requirements.xlsx
+++ b/doc/requirements.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$70</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$72</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="151">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -79,7 +79,9 @@
     <t xml:space="preserve">rq_excl_id</t>
   </si>
   <si>
-    <t xml:space="preserve">VRM2 shall enable exclusion of requirements from diagram based on &lt;id&gt;</t>
+    <t xml:space="preserve">VRM2 shall enable exclusion of requirements from diagram based on &lt;id&gt; and in case of duplicate &lt;id&gt;s the key created from id:version.
+Comment: exclusion is typically done interactively, where the relevant identifier is picked up programatically with a right-click on relevant requirement.
+</t>
   </si>
   <si>
     <t xml:space="preserve">rq_doctype_color</t>
@@ -466,7 +468,23 @@
     <t xml:space="preserve">VRM2 shall provide drag-and-drop for reference oreqm file</t>
   </si>
   <si>
-    <t xml:space="preserve">VRM2 shall </t>
+    <t xml:space="preserve">rq_dup_req</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall handle duplicate ids and calculate links based on id+version
+If no matching version is found for a fulfilledby or coverage relation, it is unspecified which duplicate is linked to.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_dup_req_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall handle group duplicate requirements together visually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_dup_same_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall log an issue when a non-unique id+version pair is detected</t>
   </si>
 </sst>
 </file>
@@ -813,13 +831,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -853,7 +871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -870,7 +888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -887,7 +905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -921,7 +939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>17</v>
       </c>
@@ -938,7 +956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -955,7 +973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
@@ -972,7 +990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>23</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>25</v>
       </c>
@@ -1023,7 +1041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>29</v>
       </c>
@@ -1040,7 +1058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>31</v>
       </c>
@@ -1057,7 +1075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>33</v>
       </c>
@@ -1074,7 +1092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>35</v>
       </c>
@@ -1091,7 +1109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>37</v>
       </c>
@@ -1108,7 +1126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>39</v>
       </c>
@@ -1125,7 +1143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>41</v>
       </c>
@@ -1142,7 +1160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>43</v>
       </c>
@@ -1159,7 +1177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>45</v>
       </c>
@@ -1176,7 +1194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>47</v>
       </c>
@@ -1193,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>49</v>
       </c>
@@ -1210,7 +1228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>51</v>
       </c>
@@ -1227,7 +1245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>53</v>
       </c>
@@ -1244,7 +1262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>55</v>
       </c>
@@ -1261,7 +1279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>57</v>
       </c>
@@ -1278,7 +1296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>59</v>
       </c>
@@ -1295,7 +1313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>61</v>
       </c>
@@ -1329,7 +1347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>65</v>
       </c>
@@ -1346,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>67</v>
       </c>
@@ -1363,7 +1381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>69</v>
       </c>
@@ -1380,7 +1398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>71</v>
       </c>
@@ -1397,7 +1415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>73</v>
       </c>
@@ -1414,7 +1432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>75</v>
       </c>
@@ -1431,7 +1449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>77</v>
       </c>
@@ -1448,7 +1466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>79</v>
       </c>
@@ -1465,7 +1483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>81</v>
       </c>
@@ -1482,7 +1500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>83</v>
       </c>
@@ -1499,7 +1517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>85</v>
       </c>
@@ -1516,7 +1534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>87</v>
       </c>
@@ -1533,7 +1551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>89</v>
       </c>
@@ -1550,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>91</v>
       </c>
@@ -1567,7 +1585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>93</v>
       </c>
@@ -1584,7 +1602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>95</v>
       </c>
@@ -1601,7 +1619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>97</v>
       </c>
@@ -1635,7 +1653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>101</v>
       </c>
@@ -1652,7 +1670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>103</v>
       </c>
@@ -1669,7 +1687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>105</v>
       </c>
@@ -1686,7 +1704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="24" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>107</v>
       </c>
@@ -1703,7 +1721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>109</v>
       </c>
@@ -1720,7 +1738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>111</v>
       </c>
@@ -1737,7 +1755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>113</v>
       </c>
@@ -1754,7 +1772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>115</v>
       </c>
@@ -1771,7 +1789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>117</v>
       </c>
@@ -1788,7 +1806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="24" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>119</v>
       </c>
@@ -1805,7 +1823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>121</v>
       </c>
@@ -1822,7 +1840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="46" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>123</v>
       </c>
@@ -1856,7 +1874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>127</v>
       </c>
@@ -1873,7 +1891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>129</v>
       </c>
@@ -1890,7 +1908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>131</v>
       </c>
@@ -1907,7 +1925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>133</v>
       </c>
@@ -1924,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>135</v>
       </c>
@@ -1941,7 +1959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>137</v>
       </c>
@@ -1958,7 +1976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>139</v>
       </c>
@@ -1975,7 +1993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>141</v>
       </c>
@@ -1992,7 +2010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>143</v>
       </c>
@@ -2009,13 +2027,70 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="24" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="D70" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G70"/>
+  <autoFilter ref="A1:G72">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="VRM2 shall calculate the set of shown requirements based on reachability from selected requirements through coverage relations.&#10;Excluded ids shall stop the graph traversal and thus limit the set of shown requirements.&#10;Excluded doctypes shall stop the graph traversal and thus limit the set of shown requirements."/>
+        <filter val="VRM2 shall display a legend containing input file name(s), selection criteria, excluded ids and ‘safety’ rules, i.e. the information needed to reproduce the diagram."/>
+        <filter val="VRM2 shall enable exclusion of requirements from diagram based on &lt;id&gt;"/>
+        <filter val="VRM2 shall enable exclusion of requirements from diagram based on doctypes"/>
+        <filter val="VRM2 shall provide a mechanism to exclude ‘rejected’ requirements from the diagram"/>
+        <filter val="VRM2 shall provide an option to exclude a specobject from the context menu"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Updated requirements. Removed log message
</commit_message>
<xml_diff>
--- a/doc/requirements.xlsx
+++ b/doc/requirements.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$72</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="159">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -481,10 +482,36 @@
     <t xml:space="preserve">VRM2 shall handle group duplicate requirements together visually</t>
   </si>
   <si>
+    <t xml:space="preserve">rq_dup_req_setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall have a setting for grouping and highlighting duplicates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_dup_req_search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall have a mechanism to search for duplicate requirement from 'Selection criteria' box.</t>
+  </si>
+  <si>
     <t xml:space="preserve">rq_dup_same_version</t>
   </si>
   <si>
     <t xml:space="preserve">VRM2 shall log an issue when a non-unique id+version pair is detected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_markup_remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall have a mechanism to remove markup from display specobject texts.
+Comment: graphviz is unable to render docbook or html markup, so remove is essential for readable requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_automatic_diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall be able to generate diagrams (requirements, hierarchy, safety) from the command line, without a window being displayed, and with all relevant pameters specified on the command line.
+Comment: This feature is intended for CI where automatic generation of a diagram is desirable.</t>
   </si>
 </sst>
 </file>
@@ -499,6 +526,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -516,29 +544,34 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -546,6 +579,36 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -553,50 +616,28 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -605,30 +646,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -646,6 +663,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -697,23 +738,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -744,23 +819,23 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -831,19 +906,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="102.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.72"/>
   </cols>
@@ -871,7 +946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -888,7 +963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -905,7 +980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -956,7 +1031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -973,7 +1048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
@@ -990,7 +1065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>23</v>
       </c>
@@ -1007,7 +1082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>25</v>
       </c>
@@ -1041,7 +1116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>29</v>
       </c>
@@ -1058,7 +1133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>31</v>
       </c>
@@ -1075,7 +1150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>33</v>
       </c>
@@ -1092,7 +1167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>35</v>
       </c>
@@ -1109,7 +1184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>37</v>
       </c>
@@ -1126,7 +1201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>39</v>
       </c>
@@ -1143,7 +1218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>41</v>
       </c>
@@ -1160,7 +1235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>43</v>
       </c>
@@ -1177,7 +1252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>45</v>
       </c>
@@ -1194,7 +1269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>47</v>
       </c>
@@ -1211,7 +1286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>49</v>
       </c>
@@ -1228,7 +1303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>51</v>
       </c>
@@ -1245,7 +1320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>53</v>
       </c>
@@ -1262,7 +1337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>55</v>
       </c>
@@ -1279,7 +1354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>57</v>
       </c>
@@ -1296,7 +1371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>59</v>
       </c>
@@ -1313,7 +1388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>61</v>
       </c>
@@ -1347,7 +1422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>65</v>
       </c>
@@ -1364,7 +1439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>67</v>
       </c>
@@ -1381,7 +1456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>69</v>
       </c>
@@ -1398,7 +1473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>71</v>
       </c>
@@ -1415,7 +1490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>73</v>
       </c>
@@ -1432,7 +1507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>75</v>
       </c>
@@ -1449,7 +1524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>77</v>
       </c>
@@ -1466,7 +1541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>79</v>
       </c>
@@ -1483,7 +1558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>81</v>
       </c>
@@ -1500,7 +1575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>83</v>
       </c>
@@ -1517,7 +1592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>85</v>
       </c>
@@ -1534,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>87</v>
       </c>
@@ -1551,7 +1626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>89</v>
       </c>
@@ -1568,7 +1643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>91</v>
       </c>
@@ -1585,7 +1660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>93</v>
       </c>
@@ -1602,7 +1677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>95</v>
       </c>
@@ -1619,7 +1694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>97</v>
       </c>
@@ -1653,7 +1728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>101</v>
       </c>
@@ -1670,7 +1745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>103</v>
       </c>
@@ -1687,7 +1762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>105</v>
       </c>
@@ -1704,7 +1779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="24" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>107</v>
       </c>
@@ -1721,7 +1796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>109</v>
       </c>
@@ -1738,7 +1813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>111</v>
       </c>
@@ -1755,7 +1830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>113</v>
       </c>
@@ -1772,7 +1847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>115</v>
       </c>
@@ -1789,7 +1864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>117</v>
       </c>
@@ -1806,7 +1881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="24" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>119</v>
       </c>
@@ -1823,7 +1898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>121</v>
       </c>
@@ -1840,7 +1915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="46" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>123</v>
       </c>
@@ -1874,7 +1949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>127</v>
       </c>
@@ -1891,7 +1966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>129</v>
       </c>
@@ -1908,7 +1983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>131</v>
       </c>
@@ -1925,7 +2000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>133</v>
       </c>
@@ -1942,7 +2017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>135</v>
       </c>
@@ -1959,7 +2034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>137</v>
       </c>
@@ -1976,7 +2051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>139</v>
       </c>
@@ -1993,7 +2068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>141</v>
       </c>
@@ -2010,7 +2085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>143</v>
       </c>
@@ -2027,7 +2102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="24" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>145</v>
       </c>
@@ -2044,7 +2119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>147</v>
       </c>
@@ -2061,7 +2136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>149</v>
       </c>
@@ -2078,19 +2153,76 @@
         <v>10</v>
       </c>
     </row>
+    <row r="73" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G72">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="VRM2 shall calculate the set of shown requirements based on reachability from selected requirements through coverage relations.&#10;Excluded ids shall stop the graph traversal and thus limit the set of shown requirements.&#10;Excluded doctypes shall stop the graph traversal and thus limit the set of shown requirements."/>
-        <filter val="VRM2 shall display a legend containing input file name(s), selection criteria, excluded ids and ‘safety’ rules, i.e. the information needed to reproduce the diagram."/>
-        <filter val="VRM2 shall enable exclusion of requirements from diagram based on &lt;id&gt;"/>
-        <filter val="VRM2 shall enable exclusion of requirements from diagram based on doctypes"/>
-        <filter val="VRM2 shall provide a mechanism to exclude ‘rejected’ requirements from the diagram"/>
-        <filter val="VRM2 shall provide an option to exclude a specobject from the context menu"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G76"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
changed doctypes to built-in defaults
</commit_message>
<xml_diff>
--- a/doc/requirements.xlsx
+++ b/doc/requirements.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$74</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">VRM2 shall read requirements from .oreqm files</t>
   </si>
   <si>
-    <t xml:space="preserve">impl;test</t>
+    <t xml:space="preserve">sourcecode;testcode</t>
   </si>
   <si>
     <t xml:space="preserve">rq_dot</t>
@@ -912,13 +912,13 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="102.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.72"/>
   </cols>

</xml_diff>

<commit_message>
some requirements are non-functional. Update reqm2 script
</commit_message>
<xml_diff>
--- a/doc/requirements.xlsx
+++ b/doc/requirements.xlsx
@@ -8,11 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="requirements" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="nonfunctional" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$74</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">requirements!$A$1:$G$72</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">requirements!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="159">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -364,30 +365,6 @@
     <t xml:space="preserve">VRM2 shall provide a mechanism for automatic software update on Windows.</t>
   </si>
   <si>
-    <t xml:space="preserve">rq_linux_installable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VRM2 shall provide installable executables for Linux with association to .oreqm filetype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rq_linux_stand_alone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VRM2 shall provide stand-alone executables for Linux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rq_win_stand_alone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VRM2 shall provide stand-alone executable for Windows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rq_win_installable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VRM2 shall provide installable executable for Windows with association to .oreqm filetype</t>
-  </si>
-  <si>
     <t xml:space="preserve">rq_config_node_limit</t>
   </si>
   <si>
@@ -510,8 +487,32 @@
     <t xml:space="preserve">rq_automatic_diagram</t>
   </si>
   <si>
-    <t xml:space="preserve">VRM2 shall be able to generate diagrams (requirements, hierarchy, safety) from the command line, without a window being displayed, and with all relevant pameters specified on the command line.
+    <t xml:space="preserve">VRM2 shall be able to generate diagrams (requirements, hierarchy, safety) from the command line and with all relevant pameters specified on the command line.
 Comment: This feature is intended for CI where automatic generation of a diagram is desirable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_linux_installable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall provide installable executables for Linux with association to .oreqm filetype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_linux_stand_alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall provide stand-alone executables for Linux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_win_stand_alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall provide stand-alone executable for Windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_win_installable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall provide installable executable for Windows with association to .oreqm filetype</t>
   </si>
 </sst>
 </file>
@@ -909,13 +910,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.11"/>
@@ -1813,7 +1814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>111</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>115</v>
       </c>
@@ -1864,7 +1865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>117</v>
       </c>
@@ -1881,7 +1882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>119</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>123</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>125</v>
       </c>
@@ -2034,7 +2035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>137</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>145</v>
       </c>
@@ -2119,7 +2120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>147</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>149</v>
       </c>
@@ -2153,76 +2154,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B73" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B75" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B76" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G76"/>
+  <autoFilter ref="A1:G72"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2232,4 +2165,119 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update requirements - fs.watch
</commit_message>
<xml_diff>
--- a/doc/requirements.xlsx
+++ b/doc/requirements.xlsx
@@ -12,9 +12,9 @@
     <sheet name="nonfunctional" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">requirements!$A$1:$H$76</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">requirements!$A$1:$G$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">requirements!$A$1:$G$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">requirements!$A$1:$G$74</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">requirements!$A$1:$H$76</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="171">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t xml:space="preserve">VRM2 shall visualize changed linksto and fulfilledby references in comparisons. I,e, old edge has a distinct appearance. Version updates to non-duplicated requirements are not considered changed references.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_watch_files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall monitor loaded oreqm files for changes and via a popup offer to reload the file.</t>
   </si>
   <si>
     <t xml:space="preserve">rq_linux_installable</t>
@@ -945,10 +951,10 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H48" activeCellId="0" sqref="H48"/>
+      <selection pane="topLeft" activeCell="E77" activeCellId="0" sqref="E77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.11"/>
@@ -2272,9 +2278,29 @@
         <v>126</v>
       </c>
     </row>
+    <row r="77" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:H76"/>
+  <autoFilter ref="A1:G74"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2297,7 +2323,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2324,7 +2350,7 @@
     </row>
     <row r="2" customFormat="false" ht="100" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2333,7 +2359,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>11</v>
@@ -2341,7 +2367,7 @@
     </row>
     <row r="3" customFormat="false" ht="62.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -2350,7 +2376,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
@@ -2358,7 +2384,7 @@
     </row>
     <row r="4" customFormat="false" ht="62.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -2367,7 +2393,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>11</v>
@@ -2375,7 +2401,7 @@
     </row>
     <row r="5" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -2384,7 +2410,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fix req type. Add reqs for xlsx export and VQL functions
</commit_message>
<xml_diff>
--- a/doc/requirements.xlsx
+++ b/doc/requirements.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="193">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -540,16 +540,58 @@
     <t xml:space="preserve">VRM2 shall offer a mechanism to get a line separated list of selected nodes on the clipboard as text.</t>
   </si>
   <si>
-    <t xml:space="preserve">rg_table_search</t>
+    <t xml:space="preserve">rq_table_search</t>
   </si>
   <si>
     <t xml:space="preserve">VRM2 shall offer a ‘find’ functionality in the table view.</t>
   </si>
   <si>
-    <t xml:space="preserve">rg_single_view</t>
+    <t xml:space="preserve">rq_single_view</t>
   </si>
   <si>
     <t xml:space="preserve">VRM2 shall offer an option to create a diagram where only one of the selected nodes is used to generate the diagram. This can make it possible to examine otherwise too big selections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_spreadsheet_export</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall offer the option to export the selected specobjects to a spreadsheet file in xlsx format. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_spreadsheet_export_cfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall offer user selection of specobjects fields and their order in exported file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_vql_parents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall have a VQL function that finds the set of parent specobjects from a selection set, and aplies a specified filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_vql_children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall have a VQL function that finds the set of children specobjects from a selection set, and aplies a specified filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_vql_descendants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall have a VQL function that finds the set of descendant specobjects from a selection set, and aplies a specified filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_vql_ancestors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall have a VQL function that finds the set of ancestor specobjects from a selection set, and aplies a specified filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rq_doctype_filetypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRM2 shall show the file types (from the &lt;sourcefile&gt;) that contribute to each doctype in the hierarchy view. I.e. a list of filetypes shall be added to each node in diagram.</t>
   </si>
   <si>
     <t xml:space="preserve">rq_linux_installable</t>
@@ -971,13 +1013,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C83" activeCellId="0" sqref="C83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D82" activeCellId="0" sqref="D82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.11"/>
@@ -2389,8 +2431,125 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G73"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2415,7 +2574,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.63"/>
   </cols>
@@ -2445,7 +2604,7 @@
     </row>
     <row r="2" customFormat="false" ht="100" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2454,7 +2613,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>11</v>
@@ -2462,7 +2621,7 @@
     </row>
     <row r="3" customFormat="false" ht="62.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -2471,7 +2630,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
@@ -2479,7 +2638,7 @@
     </row>
     <row r="4" customFormat="false" ht="62.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -2488,7 +2647,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>11</v>
@@ -2496,7 +2655,7 @@
     </row>
     <row r="5" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -2505,7 +2664,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>11</v>

</xml_diff>